<commit_message>
ajout d'un script de nettoyage balise
</commit_message>
<xml_diff>
--- a/output_html_structure.xlsx
+++ b/output_html_structure.xlsx
@@ -473,12 +473,8 @@
   &lt;div class="main"&gt;
    &lt;div class="area"&gt;
     &lt;h1&gt;
-     Unlimited movies, TV
-     &lt;br/&gt;
-     shows, and more.
     &lt;/h1&gt;
     &lt;h3&gt;
-     Watch anywhere. Cancel anytime.
     &lt;/h3&gt;
     &lt;div class="search"&gt;
      &lt;input class="box" placeholder="Email address" type="text"/&gt;
@@ -489,21 +485,14 @@
      &lt;/span&gt;
     &lt;/div&gt;
     &lt;h4&gt;
-     Ready to watch? Enter your email to create or access your account
     &lt;/h4&gt;
    &lt;/div&gt;
   &lt;/div&gt;
   &lt;div class="container1"&gt;
    &lt;div class="text"&gt;
     &lt;h1&gt;
-     Enjoy on your TV.
     &lt;/h1&gt;
     &lt;p&gt;
-     Watchx on Smart TVs, Playstation, Xbox,
-     &lt;br/&gt;
-     Chromecast, Apple TV, Blu-ray players, and
-     &lt;br/&gt;
-     more.
     &lt;/p&gt;
    &lt;/div&gt;
    &lt;div class="image"&gt;
@@ -516,22 +505,16 @@
    &lt;/div&gt;
    &lt;div class="text"&gt;
     &lt;h1&gt;
-     Download your shows to watch on the go.
     &lt;/h1&gt;
     &lt;p&gt;
-     Save your data and watch all your favorites offline.
     &lt;/p&gt;
    &lt;/div&gt;
   &lt;/div&gt;
   &lt;div class="container1"&gt;
    &lt;div class="text"&gt;
     &lt;h1&gt;
-     Watch everywhere.
     &lt;/h1&gt;
     &lt;p&gt;
-     Stream unlimited movies and TV shows on
-     &lt;br/&gt;
-     your phone, tablet, laptop, and TV without paying more.
     &lt;/p&gt;
    &lt;/div&gt;
    &lt;div class="image"&gt;
@@ -540,7 +523,6 @@
   &lt;/div&gt;
   &lt;div class="question"&gt;
    &lt;h1&gt;
-    Frequently Asked Questions
    &lt;/h1&gt;
    &lt;div class="quest"&gt;
     &lt;div class="textbox"&gt;
@@ -593,14 +575,12 @@
     &lt;/span&gt;
    &lt;/div&gt;
    &lt;h4&gt;
-    Ready to watch? Enter your email to create or access your account
    &lt;/h4&gt;
   &lt;/div&gt;
   &lt;div class="footer"&gt;
    &lt;div class="footercon"&gt;
     &lt;div class="flex1"&gt;
      &lt;h5&gt;
-      Questions? Call 1-866-579-7172
      &lt;/h5&gt;
      &lt;h5&gt;
      &lt;/h5&gt;
@@ -608,108 +588,88 @@
     &lt;ul class="list1"&gt;
      &lt;li&gt;
       &lt;a href=""&gt;
-       FAQ
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Investor Relation
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Ways to Watch
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Corporate Information
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Netflix Originals
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
       &lt;/a&gt;
      &lt;/li&gt;
     &lt;/ul&gt;
     &lt;ul class="list1"&gt;
      &lt;li&gt;
       &lt;a href=""&gt;
-       Home
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Jobs
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Terms of Use
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Contact Us
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       #
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
       &lt;/a&gt;
      &lt;/li&gt;
     &lt;/ul&gt;
     &lt;ul class="list1"&gt;
      &lt;li&gt;
       &lt;a href=""&gt;
-       Account
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Redeem Gift Cards
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Privacy
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Speed Test
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       #
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
       &lt;/a&gt;
      &lt;/li&gt;
     &lt;/ul&gt;
     &lt;ul class="list1"&gt;
      &lt;li&gt;
       &lt;a href=""&gt;
-       Media Center&lt;&lt; /a&gt;
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Buy Gift Cards
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Cookie Preferences
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       Legal Notices
-      &lt;/a&gt;
-     &lt;/li&gt;
-     &lt;li&gt;
-      &lt;a href=""&gt;
-       #
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
+      &lt;/a&gt;
+     &lt;/li&gt;
+     &lt;li&gt;
+      &lt;a href=""&gt;
       &lt;/a&gt;
      &lt;/li&gt;
     &lt;/ul&gt;
@@ -717,7 +677,6 @@
   &lt;/div&gt;
   &lt;div class="end"&gt;
    &lt;h2&gt;
-    Netflix US
    &lt;/h2&gt;
    &lt;h2&gt;
    &lt;/h2&gt;

</xml_diff>